<commit_message>
podela po inicijalima. ttapStart:ttapEnd. csv results
</commit_message>
<xml_diff>
--- a/rezultatiProfesorovi.xlsx
+++ b/rezultatiProfesorovi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minja\OneDrive\Desktop\GIT\FingerTapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F168883D-168E-4C47-8530-89CB01DE5686}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56BB994-26E4-49B5-BDF0-AF9DE64B4F80}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F04374C7-B57D-4AB4-B52A-2EAB868DB26D}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -357,7 +357,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -365,11 +365,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -385,6 +409,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20739,7 +20770,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5F7F60D-44BA-47FF-BD29-FD7FC9404F44}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5F7F60D-44BA-47FF-BD29-FD7FC9404F44}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B18" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="35">
     <pivotField showAll="0"/>
@@ -21331,8 +21362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5009ADF9-6929-4A30-8DA1-A24EB370EE45}">
   <dimension ref="A1:BD413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="G178" sqref="G178"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21562,7 +21593,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -21609,52 +21640,69 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:44" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="14">
         <v>70.260000000000005</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="3">
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="15">
         <v>27</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="15">
         <v>0.53</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4" s="15">
         <v>0.7</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="15">
         <v>21</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="15">
         <v>4</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M4" s="15">
         <v>32</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="15">
         <v>51</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="15">
         <v>1</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="2" t="s">
+      <c r="Q4" s="17" t="s">
         <v>26</v>
       </c>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AF4" s="19"/>
+      <c r="AG4" s="19"/>
+      <c r="AH4" s="19"/>
+      <c r="AI4" s="19"/>
+      <c r="AJ4" s="19"/>
+      <c r="AO4" s="17"/>
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>